<commit_message>
radar y quitar step1 analisis
</commit_message>
<xml_diff>
--- a/project_selection_results.xlsx
+++ b/project_selection_results.xlsx
@@ -491,10 +491,10 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>72.906828</v>
+        <v>72.90652799999999</v>
       </c>
       <c r="D2" t="n">
-        <v>0.2268279999999976</v>
+        <v>0.2265279999999876</v>
       </c>
       <c r="E2" t="n">
         <v>3600</v>
@@ -529,10 +529,10 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>72.859747</v>
+        <v>72.832795</v>
       </c>
       <c r="D4" t="n">
-        <v>0.1797469999999919</v>
+        <v>0.1527949999999976</v>
       </c>
       <c r="E4" t="n">
         <v>2100</v>
@@ -603,10 +603,10 @@
         <v>22</v>
       </c>
       <c r="B2" t="n">
-        <v>72.906828</v>
+        <v>72.90652799999999</v>
       </c>
       <c r="C2" t="n">
-        <v>0.2268279999999976</v>
+        <v>0.2265279999999876</v>
       </c>
       <c r="D2" t="n">
         <v>3600</v>
@@ -642,16 +642,16 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="B5" t="n">
-        <v>72.796516</v>
+        <v>72.765146</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1165159999999901</v>
+        <v>0.08514599999999461</v>
       </c>
       <c r="D5" t="n">
-        <v>2200</v>
+        <v>2100</v>
       </c>
     </row>
   </sheetData>
@@ -700,10 +700,10 @@
         <v>22</v>
       </c>
       <c r="B2" t="n">
-        <v>72.906828</v>
+        <v>72.90652799999999</v>
       </c>
       <c r="C2" t="n">
-        <v>0.2268279999999976</v>
+        <v>0.2265279999999876</v>
       </c>
       <c r="D2" t="n">
         <v>3600</v>
@@ -711,44 +711,44 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B3" t="n">
-        <v>72.859747</v>
+        <v>72.869237</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1797469999999919</v>
+        <v>0.1892369999999914</v>
       </c>
       <c r="D3" t="n">
-        <v>2100</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="B4" t="n">
-        <v>72.81931</v>
+        <v>72.832795</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1393099999999947</v>
+        <v>0.1527949999999976</v>
       </c>
       <c r="D4" t="n">
-        <v>1200</v>
+        <v>2100</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>72.796516</v>
+        <v>72.748783</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1165159999999901</v>
+        <v>0.06878299999999626</v>
       </c>
       <c r="D5" t="n">
-        <v>2200</v>
+        <v>1200</v>
       </c>
     </row>
   </sheetData>
@@ -794,58 +794,58 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="B2" t="n">
-        <v>72.869237</v>
+        <v>72.90652799999999</v>
       </c>
       <c r="C2" t="n">
-        <v>0.1892369999999914</v>
+        <v>0.2265279999999876</v>
       </c>
       <c r="D2" t="n">
-        <v>3000</v>
+        <v>3600</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B3" t="n">
-        <v>72.859747</v>
+        <v>72.831136</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1797469999999919</v>
+        <v>0.1511359999999939</v>
       </c>
       <c r="D3" t="n">
-        <v>2100</v>
+        <v>2800</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="B4" t="n">
-        <v>72.831136</v>
+        <v>72.81931</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1511359999999939</v>
+        <v>0.1393099999999947</v>
       </c>
       <c r="D4" t="n">
-        <v>2800</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="B5" t="n">
-        <v>72.81931</v>
+        <v>72.79797600000001</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1393099999999947</v>
+        <v>0.1179759999999987</v>
       </c>
       <c r="D5" t="n">
-        <v>1200</v>
+        <v>2100</v>
       </c>
     </row>
   </sheetData>
@@ -894,10 +894,10 @@
         <v>22</v>
       </c>
       <c r="B2" t="n">
-        <v>72.906828</v>
+        <v>72.90652799999999</v>
       </c>
       <c r="C2" t="n">
-        <v>0.2268279999999976</v>
+        <v>0.2265279999999876</v>
       </c>
       <c r="D2" t="n">
         <v>3600</v>
@@ -905,16 +905,16 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B3" t="n">
-        <v>72.869237</v>
+        <v>72.832795</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1892369999999914</v>
+        <v>0.1527949999999976</v>
       </c>
       <c r="D3" t="n">
-        <v>3000</v>
+        <v>2100</v>
       </c>
     </row>
     <row r="4">
@@ -933,16 +933,16 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="B5" t="n">
-        <v>72.784015</v>
+        <v>72.794023</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1040149999999898</v>
+        <v>0.1140229999999889</v>
       </c>
       <c r="D5" t="n">
-        <v>1800</v>
+        <v>2200</v>
       </c>
     </row>
   </sheetData>
@@ -988,16 +988,16 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="B2" t="n">
-        <v>72.906828</v>
+        <v>72.869237</v>
       </c>
       <c r="C2" t="n">
-        <v>0.2268279999999976</v>
+        <v>0.1892369999999914</v>
       </c>
       <c r="D2" t="n">
-        <v>3600</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="3">
@@ -1005,10 +1005,10 @@
         <v>37</v>
       </c>
       <c r="B3" t="n">
-        <v>72.859747</v>
+        <v>72.832795</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1797469999999919</v>
+        <v>0.1527949999999976</v>
       </c>
       <c r="D3" t="n">
         <v>2100</v>
@@ -1030,13 +1030,13 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5" t="n">
-        <v>72.77908100000001</v>
+        <v>72.81931</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0990809999999982</v>
+        <v>0.1393099999999947</v>
       </c>
       <c r="D5" t="n">
         <v>1200</v>
@@ -1053,7 +1053,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1085,30 +1085,30 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="B2" t="n">
-        <v>72.859747</v>
+        <v>72.90652799999999</v>
       </c>
       <c r="C2" t="n">
-        <v>0.1797469999999919</v>
+        <v>0.2265279999999876</v>
       </c>
       <c r="D2" t="n">
-        <v>2100</v>
+        <v>3600</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B3" t="n">
-        <v>72.831136</v>
+        <v>72.832795</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1511359999999939</v>
+        <v>0.1527949999999976</v>
       </c>
       <c r="D3" t="n">
-        <v>2800</v>
+        <v>2100</v>
       </c>
     </row>
     <row r="4">
@@ -1127,30 +1127,16 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B5" t="n">
-        <v>72.796516</v>
+        <v>72.793441</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1165159999999901</v>
+        <v>0.1134409999999946</v>
       </c>
       <c r="D5" t="n">
-        <v>2200</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>19</v>
-      </c>
-      <c r="B6" t="n">
-        <v>72.74619199999999</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0.06619199999998671</v>
-      </c>
-      <c r="D6" t="n">
-        <v>1650</v>
+        <v>2800</v>
       </c>
     </row>
   </sheetData>
@@ -1199,10 +1185,10 @@
         <v>22</v>
       </c>
       <c r="B2" t="n">
-        <v>72.906828</v>
+        <v>72.90652799999999</v>
       </c>
       <c r="C2" t="n">
-        <v>0.2268279999999976</v>
+        <v>0.2265279999999876</v>
       </c>
       <c r="D2" t="n">
         <v>3600</v>
@@ -1210,16 +1196,16 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B3" t="n">
-        <v>72.859747</v>
+        <v>72.831136</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1797469999999919</v>
+        <v>0.1511359999999939</v>
       </c>
       <c r="D3" t="n">
-        <v>2100</v>
+        <v>2800</v>
       </c>
     </row>
     <row r="4">
@@ -1238,16 +1224,16 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="B5" t="n">
-        <v>72.784015</v>
+        <v>72.794023</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1040149999999898</v>
+        <v>0.1140229999999889</v>
       </c>
       <c r="D5" t="n">
-        <v>1800</v>
+        <v>2200</v>
       </c>
     </row>
   </sheetData>
@@ -1261,7 +1247,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1293,30 +1279,30 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="B2" t="n">
-        <v>72.869237</v>
+        <v>72.90652799999999</v>
       </c>
       <c r="C2" t="n">
-        <v>0.1892369999999914</v>
+        <v>0.2265279999999876</v>
       </c>
       <c r="D2" t="n">
-        <v>3000</v>
+        <v>3600</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B3" t="n">
-        <v>72.859747</v>
+        <v>72.820643</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1797469999999919</v>
+        <v>0.1406429999999972</v>
       </c>
       <c r="D3" t="n">
-        <v>2100</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="4">
@@ -1335,30 +1321,16 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="B5" t="n">
-        <v>72.752951</v>
+        <v>72.79797600000001</v>
       </c>
       <c r="C5" t="n">
-        <v>0.07295099999998911</v>
+        <v>0.1179759999999987</v>
       </c>
       <c r="D5" t="n">
-        <v>1800</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>19</v>
-      </c>
-      <c r="B6" t="n">
-        <v>72.74619199999999</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0.06619199999998671</v>
-      </c>
-      <c r="D6" t="n">
-        <v>1650</v>
+        <v>2100</v>
       </c>
     </row>
   </sheetData>
@@ -1372,7 +1344,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1404,30 +1376,30 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="B2" t="n">
-        <v>72.869237</v>
+        <v>72.90652799999999</v>
       </c>
       <c r="C2" t="n">
-        <v>0.1892369999999914</v>
+        <v>0.2265279999999876</v>
       </c>
       <c r="D2" t="n">
-        <v>3000</v>
+        <v>3600</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B3" t="n">
-        <v>72.859747</v>
+        <v>72.869237</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1797469999999919</v>
+        <v>0.1892369999999914</v>
       </c>
       <c r="D3" t="n">
-        <v>2100</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="4">
@@ -1446,30 +1418,16 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="B5" t="n">
-        <v>72.784015</v>
+        <v>72.74884</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1040149999999898</v>
+        <v>0.06883999999999446</v>
       </c>
       <c r="D5" t="n">
-        <v>1800</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>20</v>
-      </c>
-      <c r="B6" t="n">
-        <v>72.714855</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0.0348549999999932</v>
-      </c>
-      <c r="D6" t="n">
-        <v>1650</v>
+        <v>2200</v>
       </c>
     </row>
   </sheetData>
@@ -1518,10 +1476,10 @@
         <v>22</v>
       </c>
       <c r="B2" t="n">
-        <v>72.906828</v>
+        <v>72.90652799999999</v>
       </c>
       <c r="C2" t="n">
-        <v>0.2268279999999976</v>
+        <v>0.2265279999999876</v>
       </c>
       <c r="D2" t="n">
         <v>3600</v>
@@ -1529,16 +1487,16 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="B3" t="n">
-        <v>72.831136</v>
+        <v>72.869237</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1511359999999939</v>
+        <v>0.1892369999999914</v>
       </c>
       <c r="D3" t="n">
-        <v>2800</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="4">
@@ -1557,16 +1515,16 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="B5" t="n">
-        <v>72.807851</v>
+        <v>72.74799299999999</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1278509999999926</v>
+        <v>0.06799299999998709</v>
       </c>
       <c r="D5" t="n">
-        <v>2100</v>
+        <v>1800</v>
       </c>
     </row>
   </sheetData>
@@ -1617,16 +1575,16 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.7351219999999756</v>
+        <v>0.7078699999999714</v>
       </c>
       <c r="B2" t="n">
         <v>9900</v>
       </c>
       <c r="C2" t="n">
-        <v>291.455122</v>
+        <v>291.42787</v>
       </c>
       <c r="D2" t="n">
-        <v>7.425474747474501e-05</v>
+        <v>7.150202020201731e-05</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -1636,111 +1594,111 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.6970209999999781</v>
+        <v>0.6730509999999725</v>
       </c>
       <c r="B3" t="n">
-        <v>9700</v>
+        <v>9900</v>
       </c>
       <c r="C3" t="n">
-        <v>291.417021</v>
+        <v>291.393051</v>
       </c>
       <c r="D3" t="n">
-        <v>7.185783505154413e-05</v>
+        <v>6.798494949494672e-05</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>1, 22, 34, 37</t>
+          <t>1, 22, 38, 40</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.6948929999999791</v>
+        <v>0.6697689999999739</v>
       </c>
       <c r="B4" t="n">
-        <v>9900</v>
+        <v>9700</v>
       </c>
       <c r="C4" t="n">
-        <v>291.414893</v>
+        <v>291.389769</v>
       </c>
       <c r="D4" t="n">
-        <v>7.019121212121001e-05</v>
+        <v>6.904835051546123e-05</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2, 22, 37, 40</t>
+          <t>1, 22, 34, 37</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.6832259999999764</v>
+        <v>0.6690979999999627</v>
       </c>
       <c r="B5" t="n">
-        <v>9900</v>
+        <v>10000</v>
       </c>
       <c r="C5" t="n">
-        <v>291.403226</v>
+        <v>291.389098</v>
       </c>
       <c r="D5" t="n">
-        <v>6.901272727272488e-05</v>
+        <v>6.690979999999627e-05</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>1, 22, 38, 40</t>
+          <t>1, 22, 31, 40</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.6785009999999545</v>
+        <v>0.6592759999999771</v>
       </c>
       <c r="B6" t="n">
-        <v>9750</v>
+        <v>9900</v>
       </c>
       <c r="C6" t="n">
-        <v>364.078501</v>
+        <v>291.379276</v>
       </c>
       <c r="D6" t="n">
-        <v>6.958984615384149e-05</v>
+        <v>6.659353535353305e-05</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>1, 7, 19, 37, 40</t>
+          <t>1, 22, 37, 41</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.6754589999999752</v>
+        <v>0.6549609999999717</v>
       </c>
       <c r="B7" t="n">
         <v>9900</v>
       </c>
       <c r="C7" t="n">
-        <v>291.395459</v>
+        <v>291.374961</v>
       </c>
       <c r="D7" t="n">
-        <v>6.822818181817931e-05</v>
+        <v>6.615767676767391e-05</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>1, 22, 37, 41</t>
+          <t>2, 22, 37, 40</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.6735899999999759</v>
+        <v>0.6442699999999775</v>
       </c>
       <c r="B8" t="n">
         <v>9900</v>
       </c>
       <c r="C8" t="n">
-        <v>291.39359</v>
+        <v>291.36427</v>
       </c>
       <c r="D8" t="n">
-        <v>6.803939393939151e-05</v>
+        <v>6.507777777777551e-05</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -1750,225 +1708,225 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.6718909999999738</v>
+        <v>0.6402209999999684</v>
       </c>
       <c r="B9" t="n">
-        <v>10000</v>
+        <v>9900</v>
       </c>
       <c r="C9" t="n">
-        <v>291.391891</v>
+        <v>291.360221</v>
       </c>
       <c r="D9" t="n">
-        <v>6.718909999999739e-05</v>
+        <v>6.466878787878469e-05</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>1, 22, 31, 40</t>
+          <t>1, 22, 39, 40</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0.6624009999999743</v>
+        <v>0.6373429999999729</v>
       </c>
       <c r="B10" t="n">
-        <v>9100</v>
+        <v>9900</v>
       </c>
       <c r="C10" t="n">
-        <v>291.382401</v>
+        <v>291.357343</v>
       </c>
       <c r="D10" t="n">
-        <v>7.279131868131585e-05</v>
+        <v>6.437808080807807e-05</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>1, 22, 31, 37</t>
+          <t>3, 22, 37, 40</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>0.659429999999972</v>
+        <v>0.634949999999975</v>
       </c>
       <c r="B11" t="n">
-        <v>9100</v>
+        <v>9700</v>
       </c>
       <c r="C11" t="n">
-        <v>291.37943</v>
+        <v>291.35495</v>
       </c>
       <c r="D11" t="n">
-        <v>7.246483516483208e-05</v>
+        <v>6.545876288659536e-05</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>1, 34, 37, 40</t>
+          <t>1, 22, 34, 38</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>0.6593899999999735</v>
+        <v>0.6326559999999688</v>
       </c>
       <c r="B12" t="n">
-        <v>9600</v>
+        <v>9100</v>
       </c>
       <c r="C12" t="n">
-        <v>291.37939</v>
+        <v>291.352656</v>
       </c>
       <c r="D12" t="n">
-        <v>6.868645833333057e-05</v>
+        <v>6.952263736263393e-05</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>1, 7, 22, 40</t>
+          <t>1, 22, 31, 37</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>0.6567919999999816</v>
+        <v>0.6324779999999777</v>
       </c>
       <c r="B13" t="n">
-        <v>9700</v>
+        <v>9100</v>
       </c>
       <c r="C13" t="n">
-        <v>291.376792</v>
+        <v>291.352478</v>
       </c>
       <c r="D13" t="n">
-        <v>6.771051546391562e-05</v>
+        <v>6.950307692307447e-05</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>2, 22, 34, 37</t>
+          <t>1, 34, 37, 40</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>0.6529009999999573</v>
+        <v>0.6320739999999745</v>
       </c>
       <c r="B14" t="n">
-        <v>9950</v>
+        <v>9700</v>
       </c>
       <c r="C14" t="n">
-        <v>364.052901</v>
+        <v>291.352074</v>
       </c>
       <c r="D14" t="n">
-        <v>6.561819095476958e-05</v>
+        <v>6.516226804123448e-05</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>1, 19, 31, 34, 37</t>
+          <t>1, 22, 35, 37</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>0.6498999999999739</v>
+        <v>0.6309969999999652</v>
       </c>
       <c r="B15" t="n">
-        <v>8700</v>
+        <v>9800</v>
       </c>
       <c r="C15" t="n">
-        <v>291.3699</v>
+        <v>291.350997</v>
       </c>
       <c r="D15" t="n">
-        <v>7.470114942528436e-05</v>
+        <v>6.438744897958828e-05</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>1, 7, 22, 37</t>
+          <t>1, 22, 31, 34</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>0.6474369999999539</v>
+        <v>0.6244569999999783</v>
       </c>
       <c r="B16" t="n">
-        <v>9750</v>
+        <v>9900</v>
       </c>
       <c r="C16" t="n">
-        <v>364.0474369999999</v>
+        <v>291.344457</v>
       </c>
       <c r="D16" t="n">
-        <v>6.640379487179014e-05</v>
+        <v>6.307646464646245e-05</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>1, 8, 19, 37, 40</t>
+          <t>1, 22, 38, 41</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>0.647163999999961</v>
+        <v>0.6239149999999682</v>
       </c>
       <c r="B17" t="n">
-        <v>9750</v>
+        <v>10000</v>
       </c>
       <c r="C17" t="n">
-        <v>364.047164</v>
+        <v>291.343915</v>
       </c>
       <c r="D17" t="n">
-        <v>6.637579487179087e-05</v>
+        <v>6.239149999999683e-05</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>1, 7, 20, 37, 40</t>
+          <t>1, 22, 32, 40</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>0.6451249999999789</v>
+        <v>0.6230679999999609</v>
       </c>
       <c r="B18" t="n">
-        <v>9700</v>
+        <v>9600</v>
       </c>
       <c r="C18" t="n">
-        <v>291.365125</v>
+        <v>291.343068</v>
       </c>
       <c r="D18" t="n">
-        <v>6.650773195876071e-05</v>
+        <v>6.490291666666259e-05</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>1, 22, 34, 38</t>
+          <t>1, 8, 22, 40</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>0.6448889999999778</v>
+        <v>0.6205039999999684</v>
       </c>
       <c r="B19" t="n">
-        <v>9700</v>
+        <v>10000</v>
       </c>
       <c r="C19" t="n">
-        <v>291.3648889999999</v>
+        <v>291.340504</v>
       </c>
       <c r="D19" t="n">
-        <v>6.648340206185338e-05</v>
+        <v>6.205039999999685e-05</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>1, 22, 35, 37</t>
+          <t>1, 22, 31, 41</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>0.6429969999999798</v>
+        <v>0.6201419999999729</v>
       </c>
       <c r="B20" t="n">
         <v>9900</v>
       </c>
       <c r="C20" t="n">
-        <v>291.362997</v>
+        <v>291.340142</v>
       </c>
       <c r="D20" t="n">
-        <v>6.494919191918988e-05</v>
+        <v>6.264060606060332e-05</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -1978,20 +1936,20 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>0.6405209999999784</v>
+        <v>0.6168599999999742</v>
       </c>
       <c r="B21" t="n">
-        <v>9900</v>
+        <v>9700</v>
       </c>
       <c r="C21" t="n">
-        <v>291.360521</v>
+        <v>291.33686</v>
       </c>
       <c r="D21" t="n">
-        <v>6.469909090908873e-05</v>
+        <v>6.359381443298703e-05</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>1, 22, 39, 40</t>
+          <t>2, 22, 34, 37</t>
         </is>
       </c>
     </row>
@@ -2041,10 +1999,10 @@
         <v>22</v>
       </c>
       <c r="B2" t="n">
-        <v>72.906828</v>
+        <v>72.90652799999999</v>
       </c>
       <c r="C2" t="n">
-        <v>0.2268279999999976</v>
+        <v>0.2265279999999876</v>
       </c>
       <c r="D2" t="n">
         <v>3600</v>
@@ -2052,16 +2010,16 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B3" t="n">
-        <v>72.859747</v>
+        <v>72.820643</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1797469999999919</v>
+        <v>0.1406429999999972</v>
       </c>
       <c r="D3" t="n">
-        <v>2100</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="4">
@@ -2080,16 +2038,16 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B5" t="n">
-        <v>72.779004</v>
+        <v>72.794023</v>
       </c>
       <c r="C5" t="n">
-        <v>0.09900399999999365</v>
+        <v>0.1140229999999889</v>
       </c>
       <c r="D5" t="n">
-        <v>2800</v>
+        <v>2200</v>
       </c>
     </row>
   </sheetData>
@@ -2138,10 +2096,10 @@
         <v>22</v>
       </c>
       <c r="B2" t="n">
-        <v>72.906828</v>
+        <v>72.90652799999999</v>
       </c>
       <c r="C2" t="n">
-        <v>0.2268279999999976</v>
+        <v>0.2265279999999876</v>
       </c>
       <c r="D2" t="n">
         <v>3600</v>
@@ -2166,10 +2124,10 @@
         <v>38</v>
       </c>
       <c r="B4" t="n">
-        <v>72.807851</v>
+        <v>72.79797600000001</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1278509999999926</v>
+        <v>0.1179759999999987</v>
       </c>
       <c r="D4" t="n">
         <v>2100</v>
@@ -2180,10 +2138,10 @@
         <v>2</v>
       </c>
       <c r="B5" t="n">
-        <v>72.77908100000001</v>
+        <v>72.766401</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0990809999999982</v>
+        <v>0.08640099999999507</v>
       </c>
       <c r="D5" t="n">
         <v>1200</v>
@@ -2235,10 +2193,10 @@
         <v>22</v>
       </c>
       <c r="B2" t="n">
-        <v>72.906828</v>
+        <v>72.90652799999999</v>
       </c>
       <c r="C2" t="n">
-        <v>0.2268279999999976</v>
+        <v>0.2265279999999876</v>
       </c>
       <c r="D2" t="n">
         <v>3600</v>
@@ -2246,44 +2204,44 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B3" t="n">
-        <v>72.869237</v>
+        <v>72.832795</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1892369999999914</v>
+        <v>0.1527949999999976</v>
       </c>
       <c r="D3" t="n">
-        <v>3000</v>
+        <v>2100</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="B4" t="n">
-        <v>72.81931</v>
+        <v>72.831136</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1393099999999947</v>
+        <v>0.1511359999999939</v>
       </c>
       <c r="D4" t="n">
-        <v>1200</v>
+        <v>2800</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>39</v>
+        <v>2</v>
       </c>
       <c r="B5" t="n">
-        <v>72.765146</v>
+        <v>72.766401</v>
       </c>
       <c r="C5" t="n">
-        <v>0.08514599999999461</v>
+        <v>0.08640099999999507</v>
       </c>
       <c r="D5" t="n">
-        <v>2100</v>
+        <v>1200</v>
       </c>
     </row>
   </sheetData>
@@ -2332,10 +2290,10 @@
         <v>22</v>
       </c>
       <c r="B2" t="n">
-        <v>72.906828</v>
+        <v>72.90652799999999</v>
       </c>
       <c r="C2" t="n">
-        <v>0.2268279999999976</v>
+        <v>0.2265279999999876</v>
       </c>
       <c r="D2" t="n">
         <v>3600</v>
@@ -2360,10 +2318,10 @@
         <v>37</v>
       </c>
       <c r="B4" t="n">
-        <v>72.859747</v>
+        <v>72.832795</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1797469999999919</v>
+        <v>0.1527949999999976</v>
       </c>
       <c r="D4" t="n">
         <v>2100</v>
@@ -2429,10 +2387,10 @@
         <v>22</v>
       </c>
       <c r="B2" t="n">
-        <v>72.906828</v>
+        <v>72.90652799999999</v>
       </c>
       <c r="C2" t="n">
-        <v>0.2268279999999976</v>
+        <v>0.2265279999999876</v>
       </c>
       <c r="D2" t="n">
         <v>3600</v>
@@ -2440,44 +2398,44 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B3" t="n">
-        <v>72.859747</v>
+        <v>72.869237</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1797469999999919</v>
+        <v>0.1892369999999914</v>
       </c>
       <c r="D3" t="n">
-        <v>2100</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="B4" t="n">
-        <v>72.831136</v>
+        <v>72.81931</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1511359999999939</v>
+        <v>0.1393099999999947</v>
       </c>
       <c r="D4" t="n">
-        <v>2800</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="B5" t="n">
-        <v>72.81931</v>
+        <v>72.79797600000001</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1393099999999947</v>
+        <v>0.1179759999999987</v>
       </c>
       <c r="D5" t="n">
-        <v>1200</v>
+        <v>2100</v>
       </c>
     </row>
   </sheetData>
@@ -2526,10 +2484,10 @@
         <v>22</v>
       </c>
       <c r="B2" t="n">
-        <v>72.906828</v>
+        <v>72.90652799999999</v>
       </c>
       <c r="C2" t="n">
-        <v>0.2268279999999976</v>
+        <v>0.2265279999999876</v>
       </c>
       <c r="D2" t="n">
         <v>3600</v>
@@ -2537,41 +2495,41 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B3" t="n">
-        <v>72.869237</v>
+        <v>72.832795</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1892369999999914</v>
+        <v>0.1527949999999976</v>
       </c>
       <c r="D3" t="n">
-        <v>3000</v>
+        <v>2100</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B4" t="n">
-        <v>72.859747</v>
+        <v>72.831136</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1797469999999919</v>
+        <v>0.1511359999999939</v>
       </c>
       <c r="D4" t="n">
-        <v>2100</v>
+        <v>2800</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5" t="n">
-        <v>72.77908100000001</v>
+        <v>72.81931</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0990809999999982</v>
+        <v>0.1393099999999947</v>
       </c>
       <c r="D5" t="n">
         <v>1200</v>
@@ -2623,10 +2581,10 @@
         <v>22</v>
       </c>
       <c r="B2" t="n">
-        <v>72.906828</v>
+        <v>72.90652799999999</v>
       </c>
       <c r="C2" t="n">
-        <v>0.2268279999999976</v>
+        <v>0.2265279999999876</v>
       </c>
       <c r="D2" t="n">
         <v>3600</v>
@@ -2662,16 +2620,16 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B5" t="n">
-        <v>72.807851</v>
+        <v>72.794023</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1278509999999926</v>
+        <v>0.1140229999999889</v>
       </c>
       <c r="D5" t="n">
-        <v>2100</v>
+        <v>2200</v>
       </c>
     </row>
   </sheetData>
@@ -2685,7 +2643,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2717,16 +2675,16 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="B2" t="n">
-        <v>72.869237</v>
+        <v>72.90652799999999</v>
       </c>
       <c r="C2" t="n">
-        <v>0.1892369999999914</v>
+        <v>0.2265279999999876</v>
       </c>
       <c r="D2" t="n">
-        <v>3000</v>
+        <v>3600</v>
       </c>
     </row>
     <row r="3">
@@ -2734,10 +2692,10 @@
         <v>37</v>
       </c>
       <c r="B3" t="n">
-        <v>72.859747</v>
+        <v>72.832795</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1797469999999919</v>
+        <v>0.1527949999999976</v>
       </c>
       <c r="D3" t="n">
         <v>2100</v>
@@ -2745,44 +2703,30 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1</v>
+        <v>41</v>
       </c>
       <c r="B4" t="n">
-        <v>72.81931</v>
+        <v>72.820643</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1393099999999947</v>
+        <v>0.1406429999999972</v>
       </c>
       <c r="D4" t="n">
-        <v>1200</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B5" t="n">
-        <v>72.784015</v>
+        <v>72.81931</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1040149999999898</v>
+        <v>0.1393099999999947</v>
       </c>
       <c r="D5" t="n">
-        <v>1800</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>19</v>
-      </c>
-      <c r="B6" t="n">
-        <v>72.74619199999999</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0.06619199999998671</v>
-      </c>
-      <c r="D6" t="n">
-        <v>1650</v>
+        <v>1200</v>
       </c>
     </row>
   </sheetData>
@@ -2831,10 +2775,10 @@
         <v>22</v>
       </c>
       <c r="B2" t="n">
-        <v>72.906828</v>
+        <v>72.90652799999999</v>
       </c>
       <c r="C2" t="n">
-        <v>0.2268279999999976</v>
+        <v>0.2265279999999876</v>
       </c>
       <c r="D2" t="n">
         <v>3600</v>
@@ -2842,44 +2786,44 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B3" t="n">
-        <v>72.859747</v>
+        <v>72.869237</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1797469999999919</v>
+        <v>0.1892369999999914</v>
       </c>
       <c r="D3" t="n">
-        <v>2100</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="B4" t="n">
-        <v>72.81931</v>
+        <v>72.832795</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1393099999999947</v>
+        <v>0.1527949999999976</v>
       </c>
       <c r="D4" t="n">
-        <v>1200</v>
+        <v>2100</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>41</v>
+        <v>2</v>
       </c>
       <c r="B5" t="n">
-        <v>72.809574</v>
+        <v>72.766401</v>
       </c>
       <c r="C5" t="n">
-        <v>0.129573999999991</v>
+        <v>0.08640099999999507</v>
       </c>
       <c r="D5" t="n">
-        <v>3000</v>
+        <v>1200</v>
       </c>
     </row>
   </sheetData>
@@ -2939,30 +2883,30 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="B3" t="n">
-        <v>72.859747</v>
+        <v>72.842928</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1797469999999919</v>
+        <v>0.1629279999999937</v>
       </c>
       <c r="D3" t="n">
-        <v>2100</v>
+        <v>3600</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="B4" t="n">
-        <v>72.845296</v>
+        <v>72.832795</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1652959999999979</v>
+        <v>0.1527949999999976</v>
       </c>
       <c r="D4" t="n">
-        <v>3600</v>
+        <v>2100</v>
       </c>
     </row>
     <row r="5">

</xml_diff>